<commit_message>
ET styling preserved and country change feature sorted
</commit_message>
<xml_diff>
--- a/input_data.xlsx
+++ b/input_data.xlsx
@@ -116,7 +116,7 @@
     <t>https://ittech-news.com/landing_pages/servicenow/asad-example-sn.html</t>
   </si>
   <si>
-    <t>CT</t>
+    <t>Core Technology</t>
   </si>
   <si>
     <t>North</t>
@@ -230,7 +230,7 @@
     <t>OL-paid_25Q1_CAM_COBC_SPMT_VEMD_SNE_LOF_Strategicplann-GIC0003798-NOEU-EMEA-13529979674451909</t>
   </si>
   <si>
-    <t>CS</t>
+    <t>Customer Service</t>
   </si>
   <si>
     <t>Belgium;The Netherlands;Luxembourg</t>
@@ -287,7 +287,7 @@
     <t>OL-paid_25Q1_CAM_CSBC_CSMT_VEMD_SNE_LOF_ExecutiveInsig-GIC0003417-MESA-EMEA-5564235042043073</t>
   </si>
   <si>
-    <t>CSO</t>
+    <t>Customer Operations</t>
   </si>
   <si>
     <t>Central</t>
@@ -338,7 +338,7 @@
     <t>OL-paid_25Q1_CAM_CSBC_CSMT_VEMD_SNE_LOF_GartnerMarket-GIC0004856-DA-EMEA-5628535116476847</t>
   </si>
   <si>
-    <t>HR</t>
+    <t>Human Resources</t>
   </si>
   <si>
     <t>UKI</t>
@@ -1513,8 +1513,8 @@
   <sheetPr/>
   <dimension ref="A1:AA997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="15.75" customHeight="1"/>
@@ -2383,7 +2383,6 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>

</xml_diff>